<commit_message>
Make Year X Axis Plots for All Countires
</commit_message>
<xml_diff>
--- a/code/misc/TripleInteractionBySex.xlsx
+++ b/code/misc/TripleInteractionBySex.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bz22\Desktop\ComparativeMortality\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bz22\Desktop\ComparativeMortality\code\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4393E5-4F43-41F0-A86A-7D237FC9C522}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3E224A-E710-431A-8254-145A3C37429F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1881B21E-1D1C-4E85-99DF-F396210C29B0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="302">
   <si>
     <t>lnMortality_10</t>
   </si>
@@ -81,12 +81,6 @@
     <t>WestGermany</t>
   </si>
   <si>
-    <t>USDummy=0</t>
-  </si>
-  <si>
-    <t>USDummy=1</t>
-  </si>
-  <si>
     <t>20-29</t>
   </si>
   <si>
@@ -105,783 +99,9 @@
     <t>70-79</t>
   </si>
   <si>
-    <t>USDummy=0 # 10-19</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 20-29</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 30-39</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 40-49</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 50-59</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 60-69</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 70-79</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 80</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 10-19</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 20-29</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 30-39</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 40-49</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 50-59</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 60-69</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 70-79</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 80</t>
-  </si>
-  <si>
-    <t>YearDecade=1950</t>
-  </si>
-  <si>
-    <t>YearDecade=1960</t>
-  </si>
-  <si>
-    <t>YearDecade=1970</t>
-  </si>
-  <si>
-    <t>YearDecade=1980</t>
-  </si>
-  <si>
-    <t>YearDecade=1990</t>
-  </si>
-  <si>
-    <t>YearDecade=2000</t>
-  </si>
-  <si>
-    <t>YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=0 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=0 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=0 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=0 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=0 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=0 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=0 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=1 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=1 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=1 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=1 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=1 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=1 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=1 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>10-19 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>10-19 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>10-19 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>10-19 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>10-19 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>10-19 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>10-19 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>20-29 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>20-29 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>20-29 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>20-29 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>20-29 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>20-29 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>20-29 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>30-39 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>30-39 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>30-39 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>30-39 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>30-39 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>30-39 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>30-39 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>40-49 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>40-49 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>40-49 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>40-49 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>40-49 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>40-49 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>40-49 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>50-59 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>50-59 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>50-59 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>50-59 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>50-59 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>50-59 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>50-59 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>60-69 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>60-69 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>60-69 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>60-69 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>60-69 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>60-69 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>60-69 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>70-79 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>70-79 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>70-79 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>70-79 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>70-79 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>70-79 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>70-79 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>80 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>80 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>80 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>80 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>80 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>80 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>80 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 10-19 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 10-19 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 10-19 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 10-19 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 10-19 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 10-19 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 10-19 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 20-29 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 20-29 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 20-29 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 20-29 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 20-29 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 20-29 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 20-29 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 30-39 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 30-39 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 30-39 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 30-39 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 30-39 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 30-39 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 30-39 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 40-49 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 40-49 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 40-49 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 40-49 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 40-49 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 40-49 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 40-49 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 50-59 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 50-59 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 50-59 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 50-59 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 50-59 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 50-59 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 50-59 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 60-69 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 60-69 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 60-69 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 60-69 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 60-69 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 60-69 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 60-69 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 70-79 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 70-79 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 70-79 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 70-79 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 70-79 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 70-79 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 70-79 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 80 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 80 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 80 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 80 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 80 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 80 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 80 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 10-19 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 10-19 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 10-19 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 10-19 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 10-19 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 10-19 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 10-19 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 20-29 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 20-29 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 20-29 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 20-29 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 20-29 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 20-29 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 20-29 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 30-39 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 30-39 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 30-39 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 30-39 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 30-39 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 30-39 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 30-39 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 40-49 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 40-49 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 40-49 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 40-49 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 40-49 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 40-49 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 40-49 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 50-59 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 50-59 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 50-59 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 50-59 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 50-59 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 50-59 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 50-59 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 60-69 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 60-69 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 60-69 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 60-69 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 60-69 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 60-69 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 60-69 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 70-79 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 70-79 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 70-79 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 70-79 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 70-79 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 70-79 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 70-79 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 80 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 80 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 80 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 80 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 80 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 80 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 80 # YearDecade=2010</t>
-  </si>
-  <si>
     <t>LessThan10</t>
   </si>
   <si>
-    <t>USDummy=0 # LessThan10</t>
-  </si>
-  <si>
-    <t>USDummy=1 # LessThan10</t>
-  </si>
-  <si>
-    <t>YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=0 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=1 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>LessThan10 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>LessThan10 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>LessThan10 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>LessThan10 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>LessThan10 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>LessThan10 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>LessThan10 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>LessThan10 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>10-19 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>20-29 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>30-39 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>40-49 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>50-59 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>60-69 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>70-79 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>80 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=0 # LessThan10 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=0 # LessThan10 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=0 # LessThan10 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=0 # LessThan10 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=0 # LessThan10 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=0 # LessThan10 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=0 # LessThan10 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=0 # LessThan10 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 10-19 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 20-29 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 30-39 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 40-49 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 50-59 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 60-69 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 70-79 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=0 # 80 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=1 # LessThan10 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=1 # LessThan10 # YearDecade=1950</t>
-  </si>
-  <si>
-    <t>USDummy=1 # LessThan10 # YearDecade=1960</t>
-  </si>
-  <si>
-    <t>USDummy=1 # LessThan10 # YearDecade=1970</t>
-  </si>
-  <si>
-    <t>USDummy=1 # LessThan10 # YearDecade=1980</t>
-  </si>
-  <si>
-    <t>USDummy=1 # LessThan10 # YearDecade=1990</t>
-  </si>
-  <si>
-    <t>USDummy=1 # LessThan10 # YearDecade=2000</t>
-  </si>
-  <si>
-    <t>USDummy=1 # LessThan10 # YearDecade=2010</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 10-19 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 20-29 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 30-39 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 40-49 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 50-59 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 60-69 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 70-79 # YearDecade=1940</t>
-  </si>
-  <si>
-    <t>USDummy=1 # 80 # YearDecade=1940</t>
-  </si>
-  <si>
     <t>Constant</t>
   </si>
   <si>
@@ -925,6 +145,792 @@
   </si>
   <si>
     <t>LessFourCountriesFemaleNoLag</t>
+  </si>
+  <si>
+    <t>USDummy0</t>
+  </si>
+  <si>
+    <t>USDummy1</t>
+  </si>
+  <si>
+    <t>"10-19"</t>
+  </si>
+  <si>
+    <t>"80"</t>
+  </si>
+  <si>
+    <t>YearDecade1950</t>
+  </si>
+  <si>
+    <t>YearDecade1960</t>
+  </si>
+  <si>
+    <t>YearDecade1970</t>
+  </si>
+  <si>
+    <t>YearDecade1980</t>
+  </si>
+  <si>
+    <t>YearDecade1990</t>
+  </si>
+  <si>
+    <t>YearDecade2000</t>
+  </si>
+  <si>
+    <t>YearDecade2010</t>
+  </si>
+  <si>
+    <t>YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy0_10-19</t>
+  </si>
+  <si>
+    <t>USDummy0_20-29</t>
+  </si>
+  <si>
+    <t>USDummy0_30-39</t>
+  </si>
+  <si>
+    <t>USDummy0_40-49</t>
+  </si>
+  <si>
+    <t>USDummy0_50-59</t>
+  </si>
+  <si>
+    <t>USDummy0_60-69</t>
+  </si>
+  <si>
+    <t>USDummy0_70-79</t>
+  </si>
+  <si>
+    <t>USDummy0_80</t>
+  </si>
+  <si>
+    <t>USDummy1_10-19</t>
+  </si>
+  <si>
+    <t>USDummy1_20-29</t>
+  </si>
+  <si>
+    <t>USDummy1_30-39</t>
+  </si>
+  <si>
+    <t>USDummy1_40-49</t>
+  </si>
+  <si>
+    <t>USDummy1_50-59</t>
+  </si>
+  <si>
+    <t>USDummy1_60-69</t>
+  </si>
+  <si>
+    <t>USDummy1_70-79</t>
+  </si>
+  <si>
+    <t>USDummy1_80</t>
+  </si>
+  <si>
+    <t>USDummy0_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy0_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy0_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy0_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy0_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy0_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy0_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy1_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy1_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy1_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy1_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy1_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy1_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy1_YearDecade2010</t>
+  </si>
+  <si>
+    <t>10-19_YearDecade1950</t>
+  </si>
+  <si>
+    <t>10-19_YearDecade1960</t>
+  </si>
+  <si>
+    <t>10-19_YearDecade1970</t>
+  </si>
+  <si>
+    <t>10-19_YearDecade1980</t>
+  </si>
+  <si>
+    <t>10-19_YearDecade1990</t>
+  </si>
+  <si>
+    <t>10-19_YearDecade2000</t>
+  </si>
+  <si>
+    <t>10-19_YearDecade2010</t>
+  </si>
+  <si>
+    <t>20-29_YearDecade1950</t>
+  </si>
+  <si>
+    <t>20-29_YearDecade1960</t>
+  </si>
+  <si>
+    <t>20-29_YearDecade1970</t>
+  </si>
+  <si>
+    <t>20-29_YearDecade1980</t>
+  </si>
+  <si>
+    <t>20-29_YearDecade1990</t>
+  </si>
+  <si>
+    <t>20-29_YearDecade2000</t>
+  </si>
+  <si>
+    <t>20-29_YearDecade2010</t>
+  </si>
+  <si>
+    <t>30-39_YearDecade1950</t>
+  </si>
+  <si>
+    <t>30-39_YearDecade1960</t>
+  </si>
+  <si>
+    <t>30-39_YearDecade1970</t>
+  </si>
+  <si>
+    <t>30-39_YearDecade1980</t>
+  </si>
+  <si>
+    <t>30-39_YearDecade1990</t>
+  </si>
+  <si>
+    <t>30-39_YearDecade2000</t>
+  </si>
+  <si>
+    <t>30-39_YearDecade2010</t>
+  </si>
+  <si>
+    <t>40-49_YearDecade1950</t>
+  </si>
+  <si>
+    <t>40-49_YearDecade1960</t>
+  </si>
+  <si>
+    <t>40-49_YearDecade1970</t>
+  </si>
+  <si>
+    <t>40-49_YearDecade1980</t>
+  </si>
+  <si>
+    <t>40-49_YearDecade1990</t>
+  </si>
+  <si>
+    <t>40-49_YearDecade2000</t>
+  </si>
+  <si>
+    <t>40-49_YearDecade2010</t>
+  </si>
+  <si>
+    <t>50-59_YearDecade1950</t>
+  </si>
+  <si>
+    <t>50-59_YearDecade1960</t>
+  </si>
+  <si>
+    <t>50-59_YearDecade1970</t>
+  </si>
+  <si>
+    <t>50-59_YearDecade1980</t>
+  </si>
+  <si>
+    <t>50-59_YearDecade1990</t>
+  </si>
+  <si>
+    <t>50-59_YearDecade2000</t>
+  </si>
+  <si>
+    <t>50-59_YearDecade2010</t>
+  </si>
+  <si>
+    <t>60-69_YearDecade1950</t>
+  </si>
+  <si>
+    <t>60-69_YearDecade1960</t>
+  </si>
+  <si>
+    <t>60-69_YearDecade1970</t>
+  </si>
+  <si>
+    <t>60-69_YearDecade1980</t>
+  </si>
+  <si>
+    <t>60-69_YearDecade1990</t>
+  </si>
+  <si>
+    <t>60-69_YearDecade2000</t>
+  </si>
+  <si>
+    <t>60-69_YearDecade2010</t>
+  </si>
+  <si>
+    <t>70-79_YearDecade1950</t>
+  </si>
+  <si>
+    <t>70-79_YearDecade1960</t>
+  </si>
+  <si>
+    <t>70-79_YearDecade1970</t>
+  </si>
+  <si>
+    <t>70-79_YearDecade1980</t>
+  </si>
+  <si>
+    <t>70-79_YearDecade1990</t>
+  </si>
+  <si>
+    <t>70-79_YearDecade2000</t>
+  </si>
+  <si>
+    <t>70-79_YearDecade2010</t>
+  </si>
+  <si>
+    <t>80_YearDecade1950</t>
+  </si>
+  <si>
+    <t>80_YearDecade1960</t>
+  </si>
+  <si>
+    <t>80_YearDecade1970</t>
+  </si>
+  <si>
+    <t>80_YearDecade1980</t>
+  </si>
+  <si>
+    <t>80_YearDecade1990</t>
+  </si>
+  <si>
+    <t>80_YearDecade2000</t>
+  </si>
+  <si>
+    <t>80_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy0_10-19_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy0_10-19_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy0_10-19_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy0_10-19_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy0_10-19_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy0_10-19_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy0_10-19_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy0_20-29_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy0_20-29_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy0_20-29_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy0_20-29_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy0_20-29_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy0_20-29_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy0_20-29_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy0_30-39_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy0_30-39_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy0_30-39_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy0_30-39_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy0_30-39_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy0_30-39_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy0_30-39_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy0_40-49_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy0_40-49_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy0_40-49_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy0_40-49_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy0_40-49_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy0_40-49_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy0_40-49_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy0_50-59_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy0_50-59_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy0_50-59_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy0_50-59_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy0_50-59_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy0_50-59_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy0_50-59_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy0_60-69_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy0_60-69_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy0_60-69_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy0_60-69_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy0_60-69_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy0_60-69_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy0_60-69_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy0_70-79_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy0_70-79_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy0_70-79_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy0_70-79_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy0_70-79_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy0_70-79_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy0_70-79_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy0_80_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy0_80_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy0_80_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy0_80_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy0_80_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy0_80_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy0_80_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy1_10-19_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy1_10-19_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy1_10-19_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy1_10-19_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy1_10-19_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy1_10-19_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy1_10-19_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy1_20-29_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy1_20-29_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy1_20-29_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy1_20-29_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy1_20-29_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy1_20-29_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy1_20-29_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy1_30-39_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy1_30-39_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy1_30-39_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy1_30-39_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy1_30-39_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy1_30-39_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy1_30-39_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy1_40-49_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy1_40-49_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy1_40-49_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy1_40-49_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy1_40-49_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy1_40-49_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy1_40-49_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy1_50-59_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy1_50-59_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy1_50-59_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy1_50-59_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy1_50-59_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy1_50-59_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy1_50-59_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy1_60-69_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy1_60-69_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy1_60-69_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy1_60-69_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy1_60-69_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy1_60-69_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy1_60-69_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy1_70-79_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy1_70-79_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy1_70-79_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy1_70-79_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy1_70-79_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy1_70-79_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy1_70-79_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy1_80_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy1_80_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy1_80_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy1_80_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy1_80_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy1_80_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy1_80_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy0_LessThan10</t>
+  </si>
+  <si>
+    <t>USDummy1_LessThan10</t>
+  </si>
+  <si>
+    <t>USDummy0_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy1_YearDecade1940</t>
+  </si>
+  <si>
+    <t>LessThan10_YearDecade1940</t>
+  </si>
+  <si>
+    <t>LessThan10_YearDecade1950</t>
+  </si>
+  <si>
+    <t>LessThan10_YearDecade1960</t>
+  </si>
+  <si>
+    <t>LessThan10_YearDecade1970</t>
+  </si>
+  <si>
+    <t>LessThan10_YearDecade1980</t>
+  </si>
+  <si>
+    <t>LessThan10_YearDecade1990</t>
+  </si>
+  <si>
+    <t>LessThan10_YearDecade2000</t>
+  </si>
+  <si>
+    <t>LessThan10_YearDecade2010</t>
+  </si>
+  <si>
+    <t>10-19_YearDecade1940</t>
+  </si>
+  <si>
+    <t>20-29_YearDecade1940</t>
+  </si>
+  <si>
+    <t>30-39_YearDecade1940</t>
+  </si>
+  <si>
+    <t>40-49_YearDecade1940</t>
+  </si>
+  <si>
+    <t>50-59_YearDecade1940</t>
+  </si>
+  <si>
+    <t>60-69_YearDecade1940</t>
+  </si>
+  <si>
+    <t>70-79_YearDecade1940</t>
+  </si>
+  <si>
+    <t>80_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy0_LessThan10_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy0_LessThan10_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy0_LessThan10_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy0_LessThan10_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy0_LessThan10_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy0_LessThan10_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy0_LessThan10_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy0_LessThan10_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy0_10-19_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy0_20-29_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy0_30-39_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy0_40-49_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy0_50-59_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy0_60-69_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy0_70-79_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy0_80_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy1_LessThan10_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy1_LessThan10_YearDecade1950</t>
+  </si>
+  <si>
+    <t>USDummy1_LessThan10_YearDecade1960</t>
+  </si>
+  <si>
+    <t>USDummy1_LessThan10_YearDecade1970</t>
+  </si>
+  <si>
+    <t>USDummy1_LessThan10_YearDecade1980</t>
+  </si>
+  <si>
+    <t>USDummy1_LessThan10_YearDecade1990</t>
+  </si>
+  <si>
+    <t>USDummy1_LessThan10_YearDecade2000</t>
+  </si>
+  <si>
+    <t>USDummy1_LessThan10_YearDecade2010</t>
+  </si>
+  <si>
+    <t>USDummy1_10-19_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy1_20-29_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy1_30-39_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy1_40-49_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy1_50-59_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy1_60-69_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy1_70-79_YearDecade1940</t>
+  </si>
+  <si>
+    <t>USDummy1_80_YearDecade1940</t>
   </si>
 </sst>
 </file>
@@ -1279,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35AFAB9A-5D48-4296-8B85-AEEF046964E4}">
   <dimension ref="A1:KD13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="FH1" workbookViewId="0">
+      <selection activeCell="FV14" sqref="FV14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,7 +1296,7 @@
   <sheetData>
     <row r="1" spans="1:290" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>298</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1347,824 +1353,822 @@
         <v>17</v>
       </c>
       <c r="T1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="str">
-        <f>"10-19"</f>
-        <v>10-19</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>103</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>104</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>105</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>106</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>107</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>108</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>109</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>110</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>111</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>112</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>113</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>114</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>115</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>116</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>117</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>118</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>119</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>120</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>121</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>125</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>126</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>127</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>128</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>129</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>130</v>
+      </c>
+      <c r="DL1" t="s">
+        <v>131</v>
+      </c>
+      <c r="DM1" t="s">
+        <v>132</v>
+      </c>
+      <c r="DN1" t="s">
+        <v>133</v>
+      </c>
+      <c r="DO1" t="s">
+        <v>134</v>
+      </c>
+      <c r="DP1" t="s">
+        <v>135</v>
+      </c>
+      <c r="DQ1" t="s">
+        <v>136</v>
+      </c>
+      <c r="DR1" t="s">
+        <v>137</v>
+      </c>
+      <c r="DS1" t="s">
+        <v>138</v>
+      </c>
+      <c r="DT1" t="s">
+        <v>139</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>140</v>
+      </c>
+      <c r="DV1" t="s">
+        <v>141</v>
+      </c>
+      <c r="DW1" t="s">
+        <v>142</v>
+      </c>
+      <c r="DX1" t="s">
+        <v>143</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>144</v>
+      </c>
+      <c r="DZ1" t="s">
+        <v>145</v>
+      </c>
+      <c r="EA1" t="s">
+        <v>146</v>
+      </c>
+      <c r="EB1" t="s">
+        <v>147</v>
+      </c>
+      <c r="EC1" t="s">
+        <v>148</v>
+      </c>
+      <c r="ED1" t="s">
+        <v>149</v>
+      </c>
+      <c r="EE1" t="s">
+        <v>150</v>
+      </c>
+      <c r="EF1" t="s">
+        <v>151</v>
+      </c>
+      <c r="EG1" t="s">
+        <v>152</v>
+      </c>
+      <c r="EH1" t="s">
+        <v>153</v>
+      </c>
+      <c r="EI1" t="s">
+        <v>154</v>
+      </c>
+      <c r="EJ1" t="s">
+        <v>155</v>
+      </c>
+      <c r="EK1" t="s">
+        <v>156</v>
+      </c>
+      <c r="EL1" t="s">
+        <v>157</v>
+      </c>
+      <c r="EM1" t="s">
+        <v>158</v>
+      </c>
+      <c r="EN1" t="s">
+        <v>159</v>
+      </c>
+      <c r="EO1" t="s">
+        <v>160</v>
+      </c>
+      <c r="EP1" t="s">
+        <v>161</v>
+      </c>
+      <c r="EQ1" t="s">
+        <v>162</v>
+      </c>
+      <c r="ER1" t="s">
+        <v>163</v>
+      </c>
+      <c r="ES1" t="s">
+        <v>164</v>
+      </c>
+      <c r="ET1" t="s">
+        <v>165</v>
+      </c>
+      <c r="EU1" t="s">
+        <v>166</v>
+      </c>
+      <c r="EV1" t="s">
+        <v>167</v>
+      </c>
+      <c r="EW1" t="s">
+        <v>168</v>
+      </c>
+      <c r="EX1" t="s">
+        <v>169</v>
+      </c>
+      <c r="EY1" t="s">
+        <v>170</v>
+      </c>
+      <c r="EZ1" t="s">
+        <v>171</v>
+      </c>
+      <c r="FA1" t="s">
+        <v>172</v>
+      </c>
+      <c r="FB1" t="s">
+        <v>173</v>
+      </c>
+      <c r="FC1" t="s">
+        <v>174</v>
+      </c>
+      <c r="FD1" t="s">
+        <v>175</v>
+      </c>
+      <c r="FE1" t="s">
+        <v>176</v>
+      </c>
+      <c r="FF1" t="s">
+        <v>177</v>
+      </c>
+      <c r="FG1" t="s">
+        <v>178</v>
+      </c>
+      <c r="FH1" t="s">
+        <v>179</v>
+      </c>
+      <c r="FI1" t="s">
+        <v>180</v>
+      </c>
+      <c r="FJ1" t="s">
+        <v>181</v>
+      </c>
+      <c r="FK1" t="s">
+        <v>182</v>
+      </c>
+      <c r="FL1" t="s">
+        <v>183</v>
+      </c>
+      <c r="FM1" t="s">
+        <v>184</v>
+      </c>
+      <c r="FN1" t="s">
+        <v>185</v>
+      </c>
+      <c r="FO1" t="s">
+        <v>186</v>
+      </c>
+      <c r="FP1" t="s">
+        <v>187</v>
+      </c>
+      <c r="FQ1" t="s">
+        <v>188</v>
+      </c>
+      <c r="FR1" t="s">
+        <v>189</v>
+      </c>
+      <c r="FS1" t="s">
+        <v>190</v>
+      </c>
+      <c r="FT1" t="s">
+        <v>191</v>
+      </c>
+      <c r="FU1" t="s">
+        <v>192</v>
+      </c>
+      <c r="FV1" t="s">
+        <v>193</v>
+      </c>
+      <c r="FW1" t="s">
+        <v>194</v>
+      </c>
+      <c r="FX1" t="s">
+        <v>195</v>
+      </c>
+      <c r="FY1" t="s">
+        <v>196</v>
+      </c>
+      <c r="FZ1" t="s">
+        <v>197</v>
+      </c>
+      <c r="GA1" t="s">
+        <v>198</v>
+      </c>
+      <c r="GB1" t="s">
+        <v>199</v>
+      </c>
+      <c r="GC1" t="s">
+        <v>200</v>
+      </c>
+      <c r="GD1" t="s">
+        <v>201</v>
+      </c>
+      <c r="GE1" t="s">
+        <v>202</v>
+      </c>
+      <c r="GF1" t="s">
+        <v>203</v>
+      </c>
+      <c r="GG1" t="s">
+        <v>204</v>
+      </c>
+      <c r="GH1" t="s">
+        <v>205</v>
+      </c>
+      <c r="GI1" t="s">
+        <v>206</v>
+      </c>
+      <c r="GJ1" t="s">
+        <v>207</v>
+      </c>
+      <c r="GK1" t="s">
+        <v>208</v>
+      </c>
+      <c r="GL1" t="s">
+        <v>209</v>
+      </c>
+      <c r="GM1" t="s">
+        <v>210</v>
+      </c>
+      <c r="GN1" t="s">
+        <v>211</v>
+      </c>
+      <c r="GO1" t="s">
+        <v>212</v>
+      </c>
+      <c r="GP1" t="s">
+        <v>213</v>
+      </c>
+      <c r="GQ1" t="s">
+        <v>214</v>
+      </c>
+      <c r="GR1" t="s">
+        <v>215</v>
+      </c>
+      <c r="GS1" t="s">
+        <v>216</v>
+      </c>
+      <c r="GT1" t="s">
+        <v>217</v>
+      </c>
+      <c r="GU1" t="s">
+        <v>218</v>
+      </c>
+      <c r="GV1" t="s">
+        <v>219</v>
+      </c>
+      <c r="GW1" t="s">
+        <v>220</v>
+      </c>
+      <c r="GX1" t="s">
+        <v>221</v>
+      </c>
+      <c r="GY1" t="s">
+        <v>222</v>
+      </c>
+      <c r="GZ1" t="s">
+        <v>223</v>
+      </c>
+      <c r="HA1" t="s">
+        <v>224</v>
+      </c>
+      <c r="HB1" t="s">
+        <v>225</v>
+      </c>
+      <c r="HC1" t="s">
+        <v>226</v>
+      </c>
+      <c r="HD1" t="s">
+        <v>227</v>
+      </c>
+      <c r="HE1" t="s">
+        <v>228</v>
+      </c>
+      <c r="HF1" t="s">
+        <v>229</v>
+      </c>
+      <c r="HG1" t="s">
+        <v>230</v>
+      </c>
+      <c r="HH1" t="s">
+        <v>231</v>
+      </c>
+      <c r="HI1" t="s">
+        <v>232</v>
+      </c>
+      <c r="HJ1" t="s">
+        <v>233</v>
+      </c>
+      <c r="HK1" t="s">
+        <v>234</v>
+      </c>
+      <c r="HL1" t="s">
+        <v>235</v>
+      </c>
+      <c r="HM1" t="s">
+        <v>236</v>
+      </c>
+      <c r="HN1" t="s">
+        <v>237</v>
+      </c>
+      <c r="HO1" t="s">
+        <v>238</v>
+      </c>
+      <c r="HP1" t="s">
+        <v>239</v>
+      </c>
+      <c r="HQ1" t="s">
+        <v>240</v>
+      </c>
+      <c r="HR1" t="s">
+        <v>241</v>
+      </c>
+      <c r="HS1" t="s">
+        <v>242</v>
+      </c>
+      <c r="HT1" t="s">
+        <v>243</v>
+      </c>
+      <c r="HU1" t="s">
+        <v>244</v>
+      </c>
+      <c r="HV1" t="s">
+        <v>245</v>
+      </c>
+      <c r="HW1" t="s">
+        <v>246</v>
+      </c>
+      <c r="HX1" t="s">
+        <v>247</v>
+      </c>
+      <c r="HY1" t="s">
+        <v>248</v>
+      </c>
+      <c r="HZ1" t="s">
+        <v>249</v>
+      </c>
+      <c r="IA1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="IB1" t="s">
+        <v>250</v>
+      </c>
+      <c r="IC1" t="s">
+        <v>251</v>
+      </c>
+      <c r="ID1" t="s">
+        <v>51</v>
+      </c>
+      <c r="IE1" t="s">
+        <v>252</v>
+      </c>
+      <c r="IF1" t="s">
+        <v>253</v>
+      </c>
+      <c r="IG1" t="s">
+        <v>254</v>
+      </c>
+      <c r="IH1" t="s">
+        <v>255</v>
+      </c>
+      <c r="II1" t="s">
+        <v>256</v>
+      </c>
+      <c r="IJ1" t="s">
+        <v>257</v>
+      </c>
+      <c r="IK1" t="s">
+        <v>258</v>
+      </c>
+      <c r="IL1" t="s">
+        <v>259</v>
+      </c>
+      <c r="IM1" t="s">
+        <v>260</v>
+      </c>
+      <c r="IN1" t="s">
+        <v>261</v>
+      </c>
+      <c r="IO1" t="s">
+        <v>262</v>
+      </c>
+      <c r="IP1" t="s">
+        <v>263</v>
+      </c>
+      <c r="IQ1" t="s">
+        <v>264</v>
+      </c>
+      <c r="IR1" t="s">
+        <v>265</v>
+      </c>
+      <c r="IS1" t="s">
+        <v>266</v>
+      </c>
+      <c r="IT1" t="s">
+        <v>267</v>
+      </c>
+      <c r="IU1" t="s">
+        <v>268</v>
+      </c>
+      <c r="IV1" t="s">
+        <v>269</v>
+      </c>
+      <c r="IW1" t="s">
+        <v>270</v>
+      </c>
+      <c r="IX1" t="s">
+        <v>271</v>
+      </c>
+      <c r="IY1" t="s">
+        <v>272</v>
+      </c>
+      <c r="IZ1" t="s">
+        <v>273</v>
+      </c>
+      <c r="JA1" t="s">
+        <v>274</v>
+      </c>
+      <c r="JB1" t="s">
+        <v>275</v>
+      </c>
+      <c r="JC1" t="s">
+        <v>276</v>
+      </c>
+      <c r="JD1" t="s">
+        <v>277</v>
+      </c>
+      <c r="JE1" t="s">
+        <v>278</v>
+      </c>
+      <c r="JF1" t="s">
+        <v>279</v>
+      </c>
+      <c r="JG1" t="s">
+        <v>280</v>
+      </c>
+      <c r="JH1" t="s">
+        <v>281</v>
+      </c>
+      <c r="JI1" t="s">
+        <v>282</v>
+      </c>
+      <c r="JJ1" t="s">
+        <v>283</v>
+      </c>
+      <c r="JK1" t="s">
+        <v>284</v>
+      </c>
+      <c r="JL1" t="s">
+        <v>285</v>
+      </c>
+      <c r="JM1" t="s">
+        <v>286</v>
+      </c>
+      <c r="JN1" t="s">
+        <v>287</v>
+      </c>
+      <c r="JO1" t="s">
+        <v>288</v>
+      </c>
+      <c r="JP1" t="s">
+        <v>289</v>
+      </c>
+      <c r="JQ1" t="s">
+        <v>290</v>
+      </c>
+      <c r="JR1" t="s">
+        <v>291</v>
+      </c>
+      <c r="JS1" t="s">
+        <v>292</v>
+      </c>
+      <c r="JT1" t="s">
+        <v>293</v>
+      </c>
+      <c r="JU1" t="s">
+        <v>294</v>
+      </c>
+      <c r="JV1" t="s">
+        <v>295</v>
+      </c>
+      <c r="JW1" t="s">
+        <v>296</v>
+      </c>
+      <c r="JX1" t="s">
+        <v>297</v>
+      </c>
+      <c r="JY1" t="s">
+        <v>298</v>
+      </c>
+      <c r="JZ1" t="s">
+        <v>299</v>
+      </c>
+      <c r="KA1" t="s">
+        <v>300</v>
+      </c>
+      <c r="KB1" t="s">
+        <v>301</v>
+      </c>
+      <c r="KC1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" t="str">
-        <f>"80"</f>
-        <v>80</v>
-      </c>
-      <c r="AD1" t="s">
+      <c r="KD1" t="s">
         <v>26</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>48</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>72</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>73</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>74</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>75</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>76</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>77</v>
-      </c>
-      <c r="CD1" t="s">
-        <v>78</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>79</v>
-      </c>
-      <c r="CF1" t="s">
-        <v>80</v>
-      </c>
-      <c r="CG1" t="s">
-        <v>81</v>
-      </c>
-      <c r="CH1" t="s">
-        <v>82</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>83</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>84</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>85</v>
-      </c>
-      <c r="CL1" t="s">
-        <v>86</v>
-      </c>
-      <c r="CM1" t="s">
-        <v>87</v>
-      </c>
-      <c r="CN1" t="s">
-        <v>88</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>89</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>90</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>91</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>92</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>93</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>94</v>
-      </c>
-      <c r="CU1" t="s">
-        <v>95</v>
-      </c>
-      <c r="CV1" t="s">
-        <v>96</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>97</v>
-      </c>
-      <c r="CX1" t="s">
-        <v>98</v>
-      </c>
-      <c r="CY1" t="s">
-        <v>99</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>100</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>101</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>102</v>
-      </c>
-      <c r="DC1" t="s">
-        <v>103</v>
-      </c>
-      <c r="DD1" t="s">
-        <v>104</v>
-      </c>
-      <c r="DE1" t="s">
-        <v>105</v>
-      </c>
-      <c r="DF1" t="s">
-        <v>106</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>107</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>108</v>
-      </c>
-      <c r="DI1" t="s">
-        <v>109</v>
-      </c>
-      <c r="DJ1" t="s">
-        <v>110</v>
-      </c>
-      <c r="DK1" t="s">
-        <v>111</v>
-      </c>
-      <c r="DL1" t="s">
-        <v>112</v>
-      </c>
-      <c r="DM1" t="s">
-        <v>113</v>
-      </c>
-      <c r="DN1" t="s">
-        <v>114</v>
-      </c>
-      <c r="DO1" t="s">
-        <v>115</v>
-      </c>
-      <c r="DP1" t="s">
-        <v>116</v>
-      </c>
-      <c r="DQ1" t="s">
-        <v>117</v>
-      </c>
-      <c r="DR1" t="s">
-        <v>118</v>
-      </c>
-      <c r="DS1" t="s">
-        <v>119</v>
-      </c>
-      <c r="DT1" t="s">
-        <v>120</v>
-      </c>
-      <c r="DU1" t="s">
-        <v>121</v>
-      </c>
-      <c r="DV1" t="s">
-        <v>122</v>
-      </c>
-      <c r="DW1" t="s">
-        <v>123</v>
-      </c>
-      <c r="DX1" t="s">
-        <v>124</v>
-      </c>
-      <c r="DY1" t="s">
-        <v>125</v>
-      </c>
-      <c r="DZ1" t="s">
-        <v>126</v>
-      </c>
-      <c r="EA1" t="s">
-        <v>127</v>
-      </c>
-      <c r="EB1" t="s">
-        <v>128</v>
-      </c>
-      <c r="EC1" t="s">
-        <v>129</v>
-      </c>
-      <c r="ED1" t="s">
-        <v>130</v>
-      </c>
-      <c r="EE1" t="s">
-        <v>131</v>
-      </c>
-      <c r="EF1" t="s">
-        <v>132</v>
-      </c>
-      <c r="EG1" t="s">
-        <v>133</v>
-      </c>
-      <c r="EH1" t="s">
-        <v>134</v>
-      </c>
-      <c r="EI1" t="s">
-        <v>135</v>
-      </c>
-      <c r="EJ1" t="s">
-        <v>136</v>
-      </c>
-      <c r="EK1" t="s">
-        <v>137</v>
-      </c>
-      <c r="EL1" t="s">
-        <v>138</v>
-      </c>
-      <c r="EM1" t="s">
-        <v>139</v>
-      </c>
-      <c r="EN1" t="s">
-        <v>140</v>
-      </c>
-      <c r="EO1" t="s">
-        <v>141</v>
-      </c>
-      <c r="EP1" t="s">
-        <v>142</v>
-      </c>
-      <c r="EQ1" t="s">
-        <v>143</v>
-      </c>
-      <c r="ER1" t="s">
-        <v>144</v>
-      </c>
-      <c r="ES1" t="s">
-        <v>145</v>
-      </c>
-      <c r="ET1" t="s">
-        <v>146</v>
-      </c>
-      <c r="EU1" t="s">
-        <v>147</v>
-      </c>
-      <c r="EV1" t="s">
-        <v>148</v>
-      </c>
-      <c r="EW1" t="s">
-        <v>149</v>
-      </c>
-      <c r="EX1" t="s">
-        <v>150</v>
-      </c>
-      <c r="EY1" t="s">
-        <v>151</v>
-      </c>
-      <c r="EZ1" t="s">
-        <v>152</v>
-      </c>
-      <c r="FA1" t="s">
-        <v>153</v>
-      </c>
-      <c r="FB1" t="s">
-        <v>154</v>
-      </c>
-      <c r="FC1" t="s">
-        <v>155</v>
-      </c>
-      <c r="FD1" t="s">
-        <v>156</v>
-      </c>
-      <c r="FE1" t="s">
-        <v>157</v>
-      </c>
-      <c r="FF1" t="s">
-        <v>158</v>
-      </c>
-      <c r="FG1" t="s">
-        <v>159</v>
-      </c>
-      <c r="FH1" t="s">
-        <v>160</v>
-      </c>
-      <c r="FI1" t="s">
-        <v>161</v>
-      </c>
-      <c r="FJ1" t="s">
-        <v>162</v>
-      </c>
-      <c r="FK1" t="s">
-        <v>163</v>
-      </c>
-      <c r="FL1" t="s">
-        <v>164</v>
-      </c>
-      <c r="FM1" t="s">
-        <v>165</v>
-      </c>
-      <c r="FN1" t="s">
-        <v>166</v>
-      </c>
-      <c r="FO1" t="s">
-        <v>167</v>
-      </c>
-      <c r="FP1" t="s">
-        <v>168</v>
-      </c>
-      <c r="FQ1" t="s">
-        <v>169</v>
-      </c>
-      <c r="FR1" t="s">
-        <v>170</v>
-      </c>
-      <c r="FS1" t="s">
-        <v>171</v>
-      </c>
-      <c r="FT1" t="s">
-        <v>172</v>
-      </c>
-      <c r="FU1" t="s">
-        <v>173</v>
-      </c>
-      <c r="FV1" t="s">
-        <v>174</v>
-      </c>
-      <c r="FW1" t="s">
-        <v>175</v>
-      </c>
-      <c r="FX1" t="s">
-        <v>176</v>
-      </c>
-      <c r="FY1" t="s">
-        <v>177</v>
-      </c>
-      <c r="FZ1" t="s">
-        <v>178</v>
-      </c>
-      <c r="GA1" t="s">
-        <v>179</v>
-      </c>
-      <c r="GB1" t="s">
-        <v>180</v>
-      </c>
-      <c r="GC1" t="s">
-        <v>181</v>
-      </c>
-      <c r="GD1" t="s">
-        <v>182</v>
-      </c>
-      <c r="GE1" t="s">
-        <v>183</v>
-      </c>
-      <c r="GF1" t="s">
-        <v>184</v>
-      </c>
-      <c r="GG1" t="s">
-        <v>185</v>
-      </c>
-      <c r="GH1" t="s">
-        <v>186</v>
-      </c>
-      <c r="GI1" t="s">
-        <v>187</v>
-      </c>
-      <c r="GJ1" t="s">
-        <v>188</v>
-      </c>
-      <c r="GK1" t="s">
-        <v>189</v>
-      </c>
-      <c r="GL1" t="s">
-        <v>190</v>
-      </c>
-      <c r="GM1" t="s">
-        <v>191</v>
-      </c>
-      <c r="GN1" t="s">
-        <v>192</v>
-      </c>
-      <c r="GO1" t="s">
-        <v>193</v>
-      </c>
-      <c r="GP1" t="s">
-        <v>194</v>
-      </c>
-      <c r="GQ1" t="s">
-        <v>195</v>
-      </c>
-      <c r="GR1" t="s">
-        <v>196</v>
-      </c>
-      <c r="GS1" t="s">
-        <v>197</v>
-      </c>
-      <c r="GT1" t="s">
-        <v>198</v>
-      </c>
-      <c r="GU1" t="s">
-        <v>199</v>
-      </c>
-      <c r="GV1" t="s">
-        <v>200</v>
-      </c>
-      <c r="GW1" t="s">
-        <v>201</v>
-      </c>
-      <c r="GX1" t="s">
-        <v>202</v>
-      </c>
-      <c r="GY1" t="s">
-        <v>203</v>
-      </c>
-      <c r="GZ1" t="s">
-        <v>204</v>
-      </c>
-      <c r="HA1" t="s">
-        <v>205</v>
-      </c>
-      <c r="HB1" t="s">
-        <v>206</v>
-      </c>
-      <c r="HC1" t="s">
-        <v>207</v>
-      </c>
-      <c r="HD1" t="s">
-        <v>208</v>
-      </c>
-      <c r="HE1" t="s">
-        <v>209</v>
-      </c>
-      <c r="HF1" t="s">
-        <v>210</v>
-      </c>
-      <c r="HG1" t="s">
-        <v>211</v>
-      </c>
-      <c r="HH1" t="s">
-        <v>212</v>
-      </c>
-      <c r="HI1" t="s">
-        <v>213</v>
-      </c>
-      <c r="HJ1" t="s">
-        <v>214</v>
-      </c>
-      <c r="HK1" t="s">
-        <v>215</v>
-      </c>
-      <c r="HL1" t="s">
-        <v>216</v>
-      </c>
-      <c r="HM1" t="s">
-        <v>217</v>
-      </c>
-      <c r="HN1" t="s">
-        <v>218</v>
-      </c>
-      <c r="HO1" t="s">
-        <v>219</v>
-      </c>
-      <c r="HP1" t="s">
-        <v>220</v>
-      </c>
-      <c r="HQ1" t="s">
-        <v>221</v>
-      </c>
-      <c r="HR1" t="s">
-        <v>222</v>
-      </c>
-      <c r="HS1" t="s">
-        <v>223</v>
-      </c>
-      <c r="HT1" t="s">
-        <v>224</v>
-      </c>
-      <c r="HU1" t="s">
-        <v>225</v>
-      </c>
-      <c r="HV1" t="s">
-        <v>226</v>
-      </c>
-      <c r="HW1" t="s">
-        <v>227</v>
-      </c>
-      <c r="HX1" t="s">
-        <v>228</v>
-      </c>
-      <c r="HY1" t="s">
-        <v>229</v>
-      </c>
-      <c r="HZ1" t="s">
-        <v>230</v>
-      </c>
-      <c r="IA1" t="s">
-        <v>231</v>
-      </c>
-      <c r="IB1" t="s">
-        <v>232</v>
-      </c>
-      <c r="IC1" t="s">
-        <v>233</v>
-      </c>
-      <c r="ID1" t="s">
-        <v>234</v>
-      </c>
-      <c r="IE1" t="s">
-        <v>235</v>
-      </c>
-      <c r="IF1" t="s">
-        <v>236</v>
-      </c>
-      <c r="IG1" t="s">
-        <v>237</v>
-      </c>
-      <c r="IH1" t="s">
-        <v>238</v>
-      </c>
-      <c r="II1" t="s">
-        <v>239</v>
-      </c>
-      <c r="IJ1" t="s">
-        <v>240</v>
-      </c>
-      <c r="IK1" t="s">
-        <v>241</v>
-      </c>
-      <c r="IL1" t="s">
-        <v>242</v>
-      </c>
-      <c r="IM1" t="s">
-        <v>243</v>
-      </c>
-      <c r="IN1" t="s">
-        <v>244</v>
-      </c>
-      <c r="IO1" t="s">
-        <v>245</v>
-      </c>
-      <c r="IP1" t="s">
-        <v>246</v>
-      </c>
-      <c r="IQ1" t="s">
-        <v>247</v>
-      </c>
-      <c r="IR1" t="s">
-        <v>248</v>
-      </c>
-      <c r="IS1" t="s">
-        <v>249</v>
-      </c>
-      <c r="IT1" t="s">
-        <v>250</v>
-      </c>
-      <c r="IU1" t="s">
-        <v>251</v>
-      </c>
-      <c r="IV1" t="s">
-        <v>252</v>
-      </c>
-      <c r="IW1" t="s">
-        <v>253</v>
-      </c>
-      <c r="IX1" t="s">
-        <v>254</v>
-      </c>
-      <c r="IY1" t="s">
-        <v>255</v>
-      </c>
-      <c r="IZ1" t="s">
-        <v>256</v>
-      </c>
-      <c r="JA1" t="s">
-        <v>257</v>
-      </c>
-      <c r="JB1" t="s">
-        <v>258</v>
-      </c>
-      <c r="JC1" t="s">
-        <v>259</v>
-      </c>
-      <c r="JD1" t="s">
-        <v>260</v>
-      </c>
-      <c r="JE1" t="s">
-        <v>261</v>
-      </c>
-      <c r="JF1" t="s">
-        <v>262</v>
-      </c>
-      <c r="JG1" t="s">
-        <v>263</v>
-      </c>
-      <c r="JH1" t="s">
-        <v>264</v>
-      </c>
-      <c r="JI1" t="s">
-        <v>265</v>
-      </c>
-      <c r="JJ1" t="s">
-        <v>266</v>
-      </c>
-      <c r="JK1" t="s">
-        <v>267</v>
-      </c>
-      <c r="JL1" t="s">
-        <v>268</v>
-      </c>
-      <c r="JM1" t="s">
-        <v>269</v>
-      </c>
-      <c r="JN1" t="s">
-        <v>270</v>
-      </c>
-      <c r="JO1" t="s">
-        <v>271</v>
-      </c>
-      <c r="JP1" t="s">
-        <v>272</v>
-      </c>
-      <c r="JQ1" t="s">
-        <v>273</v>
-      </c>
-      <c r="JR1" t="s">
-        <v>274</v>
-      </c>
-      <c r="JS1" t="s">
-        <v>275</v>
-      </c>
-      <c r="JT1" t="s">
-        <v>276</v>
-      </c>
-      <c r="JU1" t="s">
-        <v>277</v>
-      </c>
-      <c r="JV1" t="s">
-        <v>278</v>
-      </c>
-      <c r="JW1" t="s">
-        <v>279</v>
-      </c>
-      <c r="JX1" t="s">
-        <v>280</v>
-      </c>
-      <c r="JY1" t="s">
-        <v>281</v>
-      </c>
-      <c r="JZ1" t="s">
-        <v>282</v>
-      </c>
-      <c r="KA1" t="s">
-        <v>283</v>
-      </c>
-      <c r="KB1" t="s">
-        <v>284</v>
-      </c>
-      <c r="KC1" t="s">
-        <v>285</v>
-      </c>
-      <c r="KD1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:290" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>287</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>1.823258</v>
@@ -2874,7 +2878,7 @@
     </row>
     <row r="3" spans="1:290" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>288</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>1.558829</v>
@@ -3584,7 +3588,7 @@
     </row>
     <row r="4" spans="1:290" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>1.7273879999999999</v>
@@ -4294,7 +4298,7 @@
     </row>
     <row r="5" spans="1:290" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>290</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -5160,7 +5164,7 @@
     </row>
     <row r="6" spans="1:290" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>291</v>
+        <v>31</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -6026,7 +6030,7 @@
     </row>
     <row r="7" spans="1:290" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>292</v>
+        <v>32</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -6892,7 +6896,7 @@
     </row>
     <row r="8" spans="1:290" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>293</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>1.8411360000000001</v>
@@ -7590,7 +7594,7 @@
     </row>
     <row r="9" spans="1:290" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>294</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>1.542419</v>
@@ -8288,7 +8292,7 @@
     </row>
     <row r="10" spans="1:290" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>295</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>1.7309270000000001</v>
@@ -8986,7 +8990,7 @@
     </row>
     <row r="11" spans="1:290" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>296</v>
+        <v>36</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -9840,7 +9844,7 @@
     </row>
     <row r="12" spans="1:290" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>297</v>
+        <v>37</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -10694,7 +10698,7 @@
     </row>
     <row r="13" spans="1:290" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>299</v>
+        <v>39</v>
       </c>
       <c r="D13">
         <v>0</v>

</xml_diff>